<commit_message>
Code updated 23-04-23 11:31:04
</commit_message>
<xml_diff>
--- a/Season_Trophies/88.xlsx
+++ b/Season_Trophies/88.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,17 +396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>68496</t>
+          <t>68017</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>42542275</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"同 风 雨"</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2534</t>
+          <t>2551</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>52565</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>56100131</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>♪iran†★</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3042</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>55846</t>
+          <t>66299</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>42558469</t>
+          <t>27113069</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>palyer25524836</t>
+          <t>㊥DumbSmoky</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,14 +470,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>2584</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>58972</t>
+          <t>56829</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2763</t>
+          <t>2866</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>65038</t>
+          <t>67440</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>43834954</t>
+          <t>42542275</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wuhugouyun</t>
+          <t>"同 风 雨"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2597</t>
+          <t>2562</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>65680</t>
+          <t>55760</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>27113069</t>
+          <t>42558469</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>㊥DumbSmoky</t>
+          <t>palyer25524836</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2584</t>
+          <t>2911</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>67420</t>
+          <t>65748</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>43834954</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>wuhugouyun</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2551</t>
+          <t>2595</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>96803</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>59222805</t>
+          <t>44437839</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAMILO</t>
+          <t>strangetamer828</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>1587</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>101322</t>
+          <t>53175</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>59231345</t>
+          <t>56100131</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Player-59231345</t>
+          <t>♪iran†★</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1602</t>
+          <t>3047</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>102250</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>44437839</t>
+          <t>59093405</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>strangetamer828</t>
+          <t>永恒不朽6</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1587</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>113592</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>59166269</t>
+          <t>59095922</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Player-59166269</t>
+          <t>xxxx7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1476</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>114728</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>59206405</t>
+          <t>59100545</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pro-59206405</t>
+          <t>"black dragon"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1456</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>59166269</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>Player-59166269</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1496</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>59100545</t>
+          <t>59206405</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"black dragon"</t>
+          <t>pro-59206405</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1454</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>96429</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>59093405</t>
+          <t>59222805</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>永恒不朽6</t>
+          <t>CAMILO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1742</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>59095922</t>
+          <t>59231345</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>xxxx7</t>
+          <t>Player-59231345</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1624</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>36127</t>
+          <t>41909</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Zephyr zgx"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4364</t>
+          <t>4091</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10919</t>
+          <t>57152</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5894</t>
+          <t>2854</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10716</t>
+          <t>30039</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>3649043</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>Dj6106</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5912</t>
+          <t>4724</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>13882</t>
+          <t>18151</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5605</t>
+          <t>5413</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18483</t>
+          <t>15695</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5287</t>
+          <t>5579</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18780</t>
+          <t>6617</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5271</t>
+          <t>6485</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23027</t>
+          <t>13897</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5019</t>
+          <t>5736</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>39859</t>
+          <t>9810</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4162</t>
+          <t>6147</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>59895</t>
+          <t>40254</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2733</t>
+          <t>4193</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>64849</t>
+          <t>26418</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2601</t>
+          <t>4909</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>14835</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>龍少</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5527</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>16518</t>
+          <t>21649</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>66666</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5406</t>
+          <t>5221</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>16649</t>
+          <t>16212</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5398</t>
+          <t>5542</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>17899</t>
+          <t>16751</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5318</t>
+          <t>5505</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>21477</t>
+          <t>24680</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5111</t>
+          <t>5015</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>22219</t>
+          <t>33875</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5066</t>
+          <t>4556</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>24657</t>
+          <t>65450</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4921</t>
+          <t>2601</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>28146</t>
+          <t>19129</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4740</t>
+          <t>5358</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>30960</t>
+          <t>31214</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3649043</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Dj6106</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4611</t>
+          <t>4673</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>33100</t>
+          <t>21736</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4515</t>
+          <t>5216</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>33547</t>
+          <t>12903</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>58839983</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>每逢佳节胖六斤</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4495</t>
+          <t>5849</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>34026</t>
+          <t>29387</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4473</t>
+          <t>4755</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>38374</t>
+          <t>60627</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>58408326</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>"Killer Bee"</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4243</t>
+          <t>2731</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>40777</t>
+          <t>30612</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4110</t>
+          <t>4700</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6598</t>
+          <t>46784</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,24 +1496,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>6302</t>
+          <t>3600</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>9035</t>
+          <t>13419</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>49043337</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>FanXiFang1976</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1523,24 +1523,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>6047</t>
+          <t>5787</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>13673</t>
+          <t>11659</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1550,24 +1550,24 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6019</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>13743</t>
+          <t>38893</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>49043337</t>
+          <t>50837459</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>FanXiFang1976</t>
+          <t>NINE日</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5618</t>
+          <t>4271</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>14481</t>
+          <t>42440</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5554</t>
+          <t>4050</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>17141</t>
+          <t>10747</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5365</t>
+          <t>6077</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>17662</t>
+          <t>13877</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>55317038</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>necman12345</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,24 +1658,24 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5333</t>
+          <t>5739</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20312</t>
+          <t>21786</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1685,24 +1685,24 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5184</t>
+          <t>5212</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>24863</t>
+          <t>16162</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1712,24 +1712,24 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4909</t>
+          <t>5545</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>30397</t>
+          <t>24104</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4636</t>
+          <t>5049</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>30416</t>
+          <t>16439</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>55317038</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>necman12345</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4635</t>
+          <t>5526</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>33414</t>
+          <t>41082</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>4502</t>
+          <t>4145</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>33703</t>
+          <t>21126</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4488</t>
+          <t>5247</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>33874</t>
+          <t>25741</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4481</t>
+          <t>4947</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>36565</t>
+          <t>15732</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>50837459</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NINE日</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>4340</t>
+          <t>5577</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>37228</t>
+          <t>34329</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4304</t>
+          <t>4535</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>40264</t>
+          <t>35187</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>4138</t>
+          <t>4492</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>41837</t>
+          <t>35943</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>4041</t>
+          <t>4449</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>41880</t>
+          <t>32956</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4039</t>
+          <t>4594</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>42749</t>
+          <t>41857</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3992</t>
+          <t>4095</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>43420</t>
+          <t>40031</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>59020292</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Sharnoth</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3934</t>
+          <t>4204</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>46807</t>
+          <t>39083</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3527</t>
+          <t>4259</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>56723</t>
+          <t>32952</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>58839983</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>每逢佳节胖六斤</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2844</t>
+          <t>4594</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>43036</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>59020292</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>龍少</t>
+          <t>Sharnoth</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4007</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>54328</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>41837764</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>好风光会长</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2952</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>60888</t>
+          <t>54204</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>2993</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>71285</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2502</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>36132</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>48738257</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>死亡洲际跳蛋</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4437</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>31015</t>
+          <t>92306</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4608</t>
+          <t>1972</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>35294</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>人山即是仙</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4406</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>48519</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3355</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>51962</t>
+          <t>54695</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>41837764</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>好风光会长</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3081</t>
+          <t>2964</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>54680</t>
+          <t>59977</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2933</t>
+          <t>2752</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>72193</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2490</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>91523</t>
+          <t>31659</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1972</t>
+          <t>4652</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>111655</t>
+          <t>46612</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1497</t>
+          <t>3621</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>111889</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>54941706</t>
+          <t>48738257</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>AlexMenjivar20</t>
+          <t>死亡洲际跳蛋</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,14 +2468,14 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1496</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>133824</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1226</t>
+          <t>1225</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>54941706</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>AlexMenjivar20</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1496</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>51979</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,14 +2549,14 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3126</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2583,17 +2583,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2610,17 +2610,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1525</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2664,17 +2664,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>人山即是仙</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2691,7 +2691,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2718,7 +2718,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2745,7 +2745,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2772,17 +2772,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>45123</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>15695258</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Player-15695258</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2792,24 +2792,24 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>3720</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>29355299</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>Player-29355299</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>41231396</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>ollsthebro</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2853,17 +2853,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>111254</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>59106471</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>anime</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1498</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>200235</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>55745105</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>eldeniz</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>192541</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>58174442</t>
+          <t>55745105</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Player-58174442</t>
+          <t>eldeniz</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2934,17 +2934,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>224374</t>
+          <t>45837</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>15695258</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Player-15695258</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>3713</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58174442</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-58174442</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3015,17 +3015,17 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>29355299</t>
+          <t>58671339</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Player-29355299</t>
+          <t>"quang pro"</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3042,17 +3042,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>58910668</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>BrittleAuthor33</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3069,17 +3069,17 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>58671339</t>
+          <t>58910668</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>"quang pro"</t>
+          <t>BrittleAuthor33</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3096,17 +3096,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>41231396</t>
+          <t>59081265</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>ollsthebro</t>
+          <t>爬楼梯</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3123,17 +3123,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>59081265</t>
+          <t>59082827</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>爬楼梯</t>
+          <t>Player-59082827</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3150,17 +3150,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>59082827</t>
+          <t>59106471</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Player-59082827</t>
+          <t>anime</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,14 +3170,14 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1498</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3196,6 +3196,249 @@
         </is>
       </c>
       <c r="E105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>71461</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>6010122</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>"Edward Peng"</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>8850180</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>30624300</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>9195340</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Namllllllik</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>69265</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>9913517</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>"Kenny Chan"</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>10636651</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>"Ismail Aflou"</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>12648101</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>"player 198827"</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>71670</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>15755724</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>"Last Good"</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>64399</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>41848598</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>国家一级保护沙雕</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>